<commit_message>
update to leadership bios
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\git\difa-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBE8358-1BB4-46DC-8497-BF7D352EB450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FC6EDB-C751-4A76-875A-D40E19154301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,10 +153,10 @@
     <t>[Tim Beatty](https://dataifa.github.io/difa-project/timothy_beatty.html)</t>
   </si>
   <si>
-    <t>[Lauren Chenarides](https://dataifa.github.io/difa-project/Leadership_team.html), [Drew Hanks](https://dataifa.github.io/difa-project/Leadership_team.html)</t>
-  </si>
-  <si>
-    <t>[Andi Carlson](https://dataifa.github.io/difa-project/Leadership_team.html)</t>
+    <t>[Lauren Chenarides](https://dataifa.github.io/difa-project/lauren_chenarides.html), [Drew Hanks](https://dataifa.github.io/difa-project/drew_hanks.html)</t>
+  </si>
+  <si>
+    <t>[Andi Carlson](https://dataifa.github.io/difa-project/andi_carlson.html)</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>